<commit_message>
Update for Road to Olympia Season 24 rules
</commit_message>
<xml_diff>
--- a/match_data/TestForm.xlsx
+++ b/match_data/TestForm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maik\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\GitHub\Legendary\match_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C5B0EDB-1A72-4D55-AD78-150D3E434002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C370BE60-8419-477B-BCA0-A37C038A6CF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Khởi động" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="44">
   <si>
     <t>KHỞI ĐỘNG</t>
   </si>
@@ -121,14 +121,7 @@
     <t>Câu hỏi phụ 3</t>
   </si>
   <si>
-    <t>Danh sách câu hỏi</t>
-  </si>
-  <si>
     <t>STT</t>
-  </si>
-  <si>
-    <t>Hướng dẫn: Nhập Câu hỏi và Đáp án tương ứng (từ trên xuống). Nhập tên file ảnh (nếu có) tương ứng với vị trí của câu hỏi.
-App sẽ tự chạy câu hỏi theo thứ tự được xác định theo "STT"</t>
   </si>
   <si>
     <t>Tên file Ảnh/Video câu hỏi</t>
@@ -165,6 +158,18 @@
   </si>
   <si>
     <t>Âm thanh</t>
+  </si>
+  <si>
+    <t>TS</t>
+  </si>
+  <si>
+    <t>PHẦN THI RIÊNG</t>
+  </si>
+  <si>
+    <t>PHẦN THI ĐỐI KHÁNG</t>
+  </si>
+  <si>
+    <t>Hướng dẫn: Nhập Câu hỏi và Đáp án tương ứng (từ trên xuống). Nhập tên file ảnh (nếu có) tương ứng với vị trí của câu hỏi.</t>
   </si>
 </sst>
 </file>
@@ -304,7 +309,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="51">
+  <borders count="54">
     <border>
       <left/>
       <right/>
@@ -821,15 +826,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color theme="0"/>
       </left>
@@ -900,12 +896,62 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="135">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -947,9 +993,6 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -971,7 +1014,7 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1004,7 +1047,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1043,9 +1086,6 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1076,16 +1116,12 @@
     <xf numFmtId="49" fontId="15" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1098,7 +1134,7 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1110,10 +1146,10 @@
     <xf numFmtId="49" fontId="15" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1128,10 +1164,10 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1170,7 +1206,7 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1185,7 +1221,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1197,16 +1233,13 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1237,7 +1270,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="13" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1255,6 +1288,48 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1475,10 +1550,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z999"/>
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1489,13 +1564,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="107" t="s">
+      <c r="A1" s="102" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="108"/>
-      <c r="C1" s="108"/>
-      <c r="D1" s="108"/>
-      <c r="E1" s="109"/>
+      <c r="B1" s="103"/>
+      <c r="C1" s="103"/>
+      <c r="D1" s="103"/>
+      <c r="E1" s="104"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -1519,13 +1594,13 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="113" t="s">
-        <v>29</v>
+      <c r="A2" s="108" t="s">
+        <v>43</v>
       </c>
-      <c r="B2" s="114"/>
-      <c r="C2" s="114"/>
-      <c r="D2" s="114"/>
-      <c r="E2" s="115"/>
+      <c r="B2" s="109"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="110"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
@@ -1549,13 +1624,13 @@
       <c r="Z2" s="2"/>
     </row>
     <row r="3" spans="1:26" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="110" t="s">
-        <v>27</v>
+      <c r="A3" s="105" t="s">
+        <v>41</v>
       </c>
-      <c r="B3" s="111"/>
-      <c r="C3" s="111"/>
-      <c r="D3" s="111"/>
-      <c r="E3" s="112"/>
+      <c r="B3" s="106"/>
+      <c r="C3" s="106"/>
+      <c r="D3" s="106"/>
+      <c r="E3" s="107"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -1580,7 +1655,7 @@
     </row>
     <row r="4" spans="1:26" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>1</v>
@@ -1617,14 +1692,14 @@
       <c r="Z4" s="1"/>
     </row>
     <row r="5" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="17">
+      <c r="A5" s="124">
         <f>ROW(A5) - 4</f>
         <v>1</v>
       </c>
-      <c r="B5" s="51"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="57"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="55"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -1648,14 +1723,11 @@
       <c r="Z5" s="1"/>
     </row>
     <row r="6" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="17">
-        <f t="shared" ref="A6:A69" si="0">ROW(A6) - 4</f>
-        <v>2</v>
-      </c>
-      <c r="B6" s="53"/>
-      <c r="C6" s="54"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="59"/>
+      <c r="A6" s="124"/>
+      <c r="B6" s="123"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="57"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -1679,14 +1751,11 @@
       <c r="Z6" s="1"/>
     </row>
     <row r="7" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="17">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="B7" s="53"/>
-      <c r="C7" s="54"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="59"/>
+      <c r="A7" s="124"/>
+      <c r="B7" s="123"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="57"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -1710,14 +1779,11 @@
       <c r="Z7" s="1"/>
     </row>
     <row r="8" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="17">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B8" s="53"/>
-      <c r="C8" s="54"/>
-      <c r="D8" s="58"/>
-      <c r="E8" s="59"/>
+      <c r="A8" s="124"/>
+      <c r="B8" s="123"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="57"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -1741,14 +1807,11 @@
       <c r="Z8" s="1"/>
     </row>
     <row r="9" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="17">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B9" s="53"/>
-      <c r="C9" s="54"/>
-      <c r="D9" s="58"/>
-      <c r="E9" s="59"/>
+      <c r="A9" s="124"/>
+      <c r="B9" s="123"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="57"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -1771,15 +1834,12 @@
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
     </row>
-    <row r="10" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="17">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B10" s="53"/>
-      <c r="C10" s="54"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="59"/>
+    <row r="10" spans="1:26" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="133"/>
+      <c r="B10" s="131"/>
+      <c r="C10" s="132"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="76"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -1803,14 +1863,13 @@
       <c r="Z10" s="1"/>
     </row>
     <row r="11" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="17">
-        <f t="shared" si="0"/>
-        <v>7</v>
+      <c r="A11" s="121">
+        <v>2</v>
       </c>
-      <c r="B11" s="53"/>
-      <c r="C11" s="54"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="59"/>
+      <c r="B11" s="129"/>
+      <c r="C11" s="130"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="74"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -1834,14 +1893,11 @@
       <c r="Z11" s="1"/>
     </row>
     <row r="12" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="17">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B12" s="53"/>
-      <c r="C12" s="54"/>
-      <c r="D12" s="58"/>
-      <c r="E12" s="59"/>
+      <c r="A12" s="121"/>
+      <c r="B12" s="51"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="57"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -1865,14 +1921,11 @@
       <c r="Z12" s="1"/>
     </row>
     <row r="13" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="17">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B13" s="53"/>
-      <c r="C13" s="54"/>
-      <c r="D13" s="58"/>
-      <c r="E13" s="59"/>
+      <c r="A13" s="121"/>
+      <c r="B13" s="51"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="57"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -1896,14 +1949,11 @@
       <c r="Z13" s="1"/>
     </row>
     <row r="14" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="17">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B14" s="53"/>
-      <c r="C14" s="54"/>
-      <c r="D14" s="58"/>
-      <c r="E14" s="59"/>
+      <c r="A14" s="121"/>
+      <c r="B14" s="51"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="57"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -1927,14 +1977,11 @@
       <c r="Z14" s="1"/>
     </row>
     <row r="15" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="17">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B15" s="55"/>
-      <c r="C15" s="55"/>
-      <c r="D15" s="58"/>
-      <c r="E15" s="59"/>
+      <c r="A15" s="121"/>
+      <c r="B15" s="53"/>
+      <c r="C15" s="53"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="57"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -1957,15 +2004,12 @@
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
     </row>
-    <row r="16" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="17">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="B16" s="55"/>
-      <c r="C16" s="55"/>
-      <c r="D16" s="58"/>
-      <c r="E16" s="59"/>
+    <row r="16" spans="1:26" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="128"/>
+      <c r="B16" s="100"/>
+      <c r="C16" s="100"/>
+      <c r="D16" s="75"/>
+      <c r="E16" s="76"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -1989,14 +2033,13 @@
       <c r="Z16" s="1"/>
     </row>
     <row r="17" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="17">
-        <f t="shared" si="0"/>
-        <v>13</v>
+      <c r="A17" s="121">
+        <v>3</v>
       </c>
-      <c r="B17" s="55"/>
-      <c r="C17" s="55"/>
-      <c r="D17" s="58"/>
-      <c r="E17" s="59"/>
+      <c r="B17" s="125"/>
+      <c r="C17" s="125"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="74"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -2020,14 +2063,11 @@
       <c r="Z17" s="1"/>
     </row>
     <row r="18" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="17">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="B18" s="55"/>
-      <c r="C18" s="55"/>
-      <c r="D18" s="60"/>
-      <c r="E18" s="60"/>
+      <c r="A18" s="121"/>
+      <c r="B18" s="53"/>
+      <c r="C18" s="53"/>
+      <c r="D18" s="58"/>
+      <c r="E18" s="58"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -2051,14 +2091,11 @@
       <c r="Z18" s="1"/>
     </row>
     <row r="19" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="17">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="B19" s="55"/>
-      <c r="C19" s="55"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="60"/>
+      <c r="A19" s="121"/>
+      <c r="B19" s="53"/>
+      <c r="C19" s="53"/>
+      <c r="D19" s="58"/>
+      <c r="E19" s="58"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -2082,14 +2119,11 @@
       <c r="Z19" s="1"/>
     </row>
     <row r="20" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="17">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="B20" s="55"/>
-      <c r="C20" s="55"/>
-      <c r="D20" s="60"/>
-      <c r="E20" s="60"/>
+      <c r="A20" s="121"/>
+      <c r="B20" s="53"/>
+      <c r="C20" s="53"/>
+      <c r="D20" s="58"/>
+      <c r="E20" s="58"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
@@ -2113,14 +2147,11 @@
       <c r="Z20" s="1"/>
     </row>
     <row r="21" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="17">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="B21" s="55"/>
-      <c r="C21" s="55"/>
-      <c r="D21" s="60"/>
-      <c r="E21" s="60"/>
+      <c r="A21" s="121"/>
+      <c r="B21" s="53"/>
+      <c r="C21" s="53"/>
+      <c r="D21" s="58"/>
+      <c r="E21" s="58"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -2143,15 +2174,12 @@
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
     </row>
-    <row r="22" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="17">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="B22" s="55"/>
-      <c r="C22" s="55"/>
-      <c r="D22" s="60"/>
-      <c r="E22" s="60"/>
+    <row r="22" spans="1:26" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="128"/>
+      <c r="B22" s="100"/>
+      <c r="C22" s="100"/>
+      <c r="D22" s="127"/>
+      <c r="E22" s="127"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -2175,14 +2203,13 @@
       <c r="Z22" s="1"/>
     </row>
     <row r="23" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="17">
-        <f t="shared" si="0"/>
-        <v>19</v>
+      <c r="A23" s="121">
+        <v>4</v>
       </c>
-      <c r="B23" s="55"/>
-      <c r="C23" s="55"/>
-      <c r="D23" s="60"/>
-      <c r="E23" s="60"/>
+      <c r="B23" s="125"/>
+      <c r="C23" s="125"/>
+      <c r="D23" s="126"/>
+      <c r="E23" s="126"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -2206,14 +2233,11 @@
       <c r="Z23" s="1"/>
     </row>
     <row r="24" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="17">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="B24" s="55"/>
-      <c r="C24" s="55"/>
-      <c r="D24" s="60"/>
-      <c r="E24" s="60"/>
+      <c r="A24" s="121"/>
+      <c r="B24" s="53"/>
+      <c r="C24" s="53"/>
+      <c r="D24" s="58"/>
+      <c r="E24" s="58"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -2237,14 +2261,11 @@
       <c r="Z24" s="1"/>
     </row>
     <row r="25" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="17">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="B25" s="55"/>
-      <c r="C25" s="55"/>
-      <c r="D25" s="60"/>
-      <c r="E25" s="60"/>
+      <c r="A25" s="121"/>
+      <c r="B25" s="53"/>
+      <c r="C25" s="53"/>
+      <c r="D25" s="58"/>
+      <c r="E25" s="58"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
@@ -2268,14 +2289,11 @@
       <c r="Z25" s="1"/>
     </row>
     <row r="26" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="17">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="B26" s="55"/>
-      <c r="C26" s="55"/>
-      <c r="D26" s="60"/>
-      <c r="E26" s="60"/>
+      <c r="A26" s="121"/>
+      <c r="B26" s="53"/>
+      <c r="C26" s="53"/>
+      <c r="D26" s="58"/>
+      <c r="E26" s="58"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
@@ -2299,14 +2317,11 @@
       <c r="Z26" s="1"/>
     </row>
     <row r="27" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="17">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="B27" s="55"/>
-      <c r="C27" s="55"/>
-      <c r="D27" s="60"/>
-      <c r="E27" s="60"/>
+      <c r="A27" s="121"/>
+      <c r="B27" s="53"/>
+      <c r="C27" s="53"/>
+      <c r="D27" s="58"/>
+      <c r="E27" s="58"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
@@ -2330,14 +2345,11 @@
       <c r="Z27" s="1"/>
     </row>
     <row r="28" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="17">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="B28" s="55"/>
-      <c r="C28" s="55"/>
-      <c r="D28" s="60"/>
-      <c r="E28" s="60"/>
+      <c r="A28" s="122"/>
+      <c r="B28" s="53"/>
+      <c r="C28" s="53"/>
+      <c r="D28" s="58"/>
+      <c r="E28" s="58"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
@@ -2360,15 +2372,14 @@
       <c r="Y28" s="1"/>
       <c r="Z28" s="1"/>
     </row>
-    <row r="29" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="17">
-        <f t="shared" si="0"/>
-        <v>25</v>
+    <row r="29" spans="1:26" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="105" t="s">
+        <v>42</v>
       </c>
-      <c r="B29" s="55"/>
-      <c r="C29" s="55"/>
-      <c r="D29" s="60"/>
-      <c r="E29" s="60"/>
+      <c r="B29" s="106"/>
+      <c r="C29" s="106"/>
+      <c r="D29" s="106"/>
+      <c r="E29" s="107"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
@@ -2391,77 +2402,82 @@
       <c r="Y29" s="1"/>
       <c r="Z29" s="1"/>
     </row>
-    <row r="30" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="17">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="B30" s="55"/>
-      <c r="C30" s="55"/>
-      <c r="D30" s="60"/>
-      <c r="E30" s="60"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3"/>
-      <c r="O30" s="3"/>
-      <c r="P30" s="3"/>
-      <c r="Q30" s="3"/>
-      <c r="R30" s="3"/>
-      <c r="S30" s="3"/>
-      <c r="T30" s="3"/>
-      <c r="U30" s="3"/>
-      <c r="V30" s="3"/>
-      <c r="W30" s="3"/>
-      <c r="X30" s="3"/>
-      <c r="Y30" s="3"/>
-      <c r="Z30" s="3"/>
-    </row>
-    <row r="31" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="17">
-        <f t="shared" si="0"/>
+    <row r="30" spans="1:26" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="55"/>
-      <c r="C31" s="55"/>
-      <c r="D31" s="60"/>
-      <c r="E31" s="60"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
-      <c r="L31" s="1"/>
-      <c r="M31" s="1"/>
-      <c r="N31" s="1"/>
-      <c r="O31" s="1"/>
-      <c r="P31" s="1"/>
-      <c r="Q31" s="1"/>
-      <c r="R31" s="1"/>
-      <c r="S31" s="1"/>
-      <c r="T31" s="1"/>
-      <c r="U31" s="1"/>
-      <c r="V31" s="1"/>
-      <c r="W31" s="1"/>
-      <c r="X31" s="1"/>
-      <c r="Y31" s="1"/>
-      <c r="Z31" s="1"/>
+      <c r="B30" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
+      <c r="S30" s="1"/>
+      <c r="T30" s="1"/>
+      <c r="U30" s="1"/>
+      <c r="V30" s="1"/>
+      <c r="W30" s="1"/>
+      <c r="X30" s="1"/>
+      <c r="Y30" s="1"/>
+      <c r="Z30" s="1"/>
+    </row>
+    <row r="31" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="16">
+        <v>1</v>
+      </c>
+      <c r="B31" s="53"/>
+      <c r="C31" s="53"/>
+      <c r="D31" s="58"/>
+      <c r="E31" s="58"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
+      <c r="P31" s="3"/>
+      <c r="Q31" s="3"/>
+      <c r="R31" s="3"/>
+      <c r="S31" s="3"/>
+      <c r="T31" s="3"/>
+      <c r="U31" s="3"/>
+      <c r="V31" s="3"/>
+      <c r="W31" s="3"/>
+      <c r="X31" s="3"/>
+      <c r="Y31" s="3"/>
+      <c r="Z31" s="3"/>
     </row>
     <row r="32" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="17">
-        <f t="shared" si="0"/>
-        <v>28</v>
+      <c r="A32" s="16">
+        <v>2</v>
       </c>
-      <c r="B32" s="55"/>
-      <c r="C32" s="55"/>
-      <c r="D32" s="60"/>
-      <c r="E32" s="60"/>
+      <c r="B32" s="53"/>
+      <c r="C32" s="53"/>
+      <c r="D32" s="58"/>
+      <c r="E32" s="58"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
@@ -2485,14 +2501,13 @@
       <c r="Z32" s="1"/>
     </row>
     <row r="33" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="17">
-        <f t="shared" si="0"/>
-        <v>29</v>
+      <c r="A33" s="16">
+        <v>3</v>
       </c>
-      <c r="B33" s="55"/>
-      <c r="C33" s="55"/>
-      <c r="D33" s="60"/>
-      <c r="E33" s="60"/>
+      <c r="B33" s="53"/>
+      <c r="C33" s="53"/>
+      <c r="D33" s="58"/>
+      <c r="E33" s="58"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
@@ -2516,14 +2531,13 @@
       <c r="Z33" s="1"/>
     </row>
     <row r="34" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="17">
-        <f t="shared" si="0"/>
-        <v>30</v>
+      <c r="A34" s="16">
+        <v>4</v>
       </c>
-      <c r="B34" s="55"/>
-      <c r="C34" s="55"/>
-      <c r="D34" s="60"/>
-      <c r="E34" s="60"/>
+      <c r="B34" s="53"/>
+      <c r="C34" s="53"/>
+      <c r="D34" s="58"/>
+      <c r="E34" s="58"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
@@ -2547,14 +2561,13 @@
       <c r="Z34" s="1"/>
     </row>
     <row r="35" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="17">
-        <f t="shared" si="0"/>
-        <v>31</v>
+      <c r="A35" s="16">
+        <v>5</v>
       </c>
-      <c r="B35" s="55"/>
-      <c r="C35" s="55"/>
-      <c r="D35" s="60"/>
-      <c r="E35" s="60"/>
+      <c r="B35" s="53"/>
+      <c r="C35" s="53"/>
+      <c r="D35" s="58"/>
+      <c r="E35" s="58"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
@@ -2578,14 +2591,13 @@
       <c r="Z35" s="1"/>
     </row>
     <row r="36" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="17">
-        <f t="shared" si="0"/>
-        <v>32</v>
+      <c r="A36" s="16">
+        <v>6</v>
       </c>
-      <c r="B36" s="55"/>
-      <c r="C36" s="55"/>
-      <c r="D36" s="60"/>
-      <c r="E36" s="60"/>
+      <c r="B36" s="53"/>
+      <c r="C36" s="53"/>
+      <c r="D36" s="58"/>
+      <c r="E36" s="58"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
@@ -2609,14 +2621,13 @@
       <c r="Z36" s="1"/>
     </row>
     <row r="37" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="17">
-        <f t="shared" si="0"/>
-        <v>33</v>
+      <c r="A37" s="16">
+        <v>7</v>
       </c>
-      <c r="B37" s="55"/>
-      <c r="C37" s="55"/>
-      <c r="D37" s="60"/>
-      <c r="E37" s="60"/>
+      <c r="B37" s="53"/>
+      <c r="C37" s="53"/>
+      <c r="D37" s="58"/>
+      <c r="E37" s="58"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
@@ -2640,14 +2651,13 @@
       <c r="Z37" s="1"/>
     </row>
     <row r="38" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="17">
-        <f t="shared" si="0"/>
-        <v>34</v>
+      <c r="A38" s="16">
+        <v>8</v>
       </c>
-      <c r="B38" s="55"/>
-      <c r="C38" s="55"/>
-      <c r="D38" s="60"/>
-      <c r="E38" s="60"/>
+      <c r="B38" s="53"/>
+      <c r="C38" s="53"/>
+      <c r="D38" s="58"/>
+      <c r="E38" s="58"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
@@ -2671,14 +2681,13 @@
       <c r="Z38" s="1"/>
     </row>
     <row r="39" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="17">
-        <f t="shared" si="0"/>
-        <v>35</v>
+      <c r="A39" s="16">
+        <v>9</v>
       </c>
-      <c r="B39" s="55"/>
-      <c r="C39" s="55"/>
-      <c r="D39" s="60"/>
-      <c r="E39" s="60"/>
+      <c r="B39" s="53"/>
+      <c r="C39" s="53"/>
+      <c r="D39" s="58"/>
+      <c r="E39" s="58"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
@@ -2702,14 +2711,13 @@
       <c r="Z39" s="1"/>
     </row>
     <row r="40" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="17">
-        <f t="shared" si="0"/>
-        <v>36</v>
+      <c r="A40" s="16">
+        <v>10</v>
       </c>
-      <c r="B40" s="55"/>
-      <c r="C40" s="55"/>
-      <c r="D40" s="60"/>
-      <c r="E40" s="60"/>
+      <c r="B40" s="53"/>
+      <c r="C40" s="53"/>
+      <c r="D40" s="58"/>
+      <c r="E40" s="58"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
@@ -2733,14 +2741,13 @@
       <c r="Z40" s="1"/>
     </row>
     <row r="41" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="17">
-        <f t="shared" si="0"/>
-        <v>37</v>
+      <c r="A41" s="16">
+        <v>11</v>
       </c>
-      <c r="B41" s="55"/>
-      <c r="C41" s="55"/>
-      <c r="D41" s="60"/>
-      <c r="E41" s="60"/>
+      <c r="B41" s="53"/>
+      <c r="C41" s="53"/>
+      <c r="D41" s="58"/>
+      <c r="E41" s="58"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
@@ -2763,15 +2770,14 @@
       <c r="Y41" s="1"/>
       <c r="Z41" s="1"/>
     </row>
-    <row r="42" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="17">
-        <f t="shared" si="0"/>
-        <v>38</v>
+    <row r="42" spans="1:26" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="134">
+        <v>12</v>
       </c>
-      <c r="B42" s="55"/>
-      <c r="C42" s="55"/>
-      <c r="D42" s="60"/>
-      <c r="E42" s="60"/>
+      <c r="B42" s="100"/>
+      <c r="C42" s="100"/>
+      <c r="D42" s="127"/>
+      <c r="E42" s="127"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
@@ -2795,14 +2801,11 @@
       <c r="Z42" s="1"/>
     </row>
     <row r="43" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="17">
-        <f t="shared" si="0"/>
-        <v>39</v>
-      </c>
-      <c r="B43" s="55"/>
-      <c r="C43" s="55"/>
-      <c r="D43" s="60"/>
-      <c r="E43" s="60"/>
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
@@ -2826,14 +2829,11 @@
       <c r="Z43" s="1"/>
     </row>
     <row r="44" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="17">
-        <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="B44" s="55"/>
-      <c r="C44" s="55"/>
-      <c r="D44" s="60"/>
-      <c r="E44" s="60"/>
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
@@ -2857,14 +2857,11 @@
       <c r="Z44" s="1"/>
     </row>
     <row r="45" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="17">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-      <c r="B45" s="55"/>
-      <c r="C45" s="55"/>
-      <c r="D45" s="60"/>
-      <c r="E45" s="60"/>
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
@@ -2888,14 +2885,11 @@
       <c r="Z45" s="1"/>
     </row>
     <row r="46" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="17">
-        <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-      <c r="B46" s="55"/>
-      <c r="C46" s="55"/>
-      <c r="D46" s="60"/>
-      <c r="E46" s="60"/>
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
@@ -2919,14 +2913,11 @@
       <c r="Z46" s="1"/>
     </row>
     <row r="47" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="17">
-        <f t="shared" si="0"/>
-        <v>43</v>
-      </c>
-      <c r="B47" s="55"/>
-      <c r="C47" s="55"/>
-      <c r="D47" s="60"/>
-      <c r="E47" s="60"/>
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
@@ -2950,14 +2941,11 @@
       <c r="Z47" s="1"/>
     </row>
     <row r="48" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="17">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-      <c r="B48" s="55"/>
-      <c r="C48" s="55"/>
-      <c r="D48" s="60"/>
-      <c r="E48" s="60"/>
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
@@ -2981,14 +2969,11 @@
       <c r="Z48" s="1"/>
     </row>
     <row r="49" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="17">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="B49" s="55"/>
-      <c r="C49" s="55"/>
-      <c r="D49" s="60"/>
-      <c r="E49" s="60"/>
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
@@ -3012,14 +2997,11 @@
       <c r="Z49" s="1"/>
     </row>
     <row r="50" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="17">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-      <c r="B50" s="55"/>
-      <c r="C50" s="55"/>
-      <c r="D50" s="60"/>
-      <c r="E50" s="60"/>
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
@@ -3043,14 +3025,11 @@
       <c r="Z50" s="1"/>
     </row>
     <row r="51" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="17">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="B51" s="55"/>
-      <c r="C51" s="55"/>
-      <c r="D51" s="60"/>
-      <c r="E51" s="60"/>
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
@@ -3074,14 +3053,11 @@
       <c r="Z51" s="1"/>
     </row>
     <row r="52" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="17">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-      <c r="B52" s="55"/>
-      <c r="C52" s="55"/>
-      <c r="D52" s="60"/>
-      <c r="E52" s="60"/>
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
@@ -3105,14 +3081,11 @@
       <c r="Z52" s="1"/>
     </row>
     <row r="53" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="17">
-        <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-      <c r="B53" s="55"/>
-      <c r="C53" s="55"/>
-      <c r="D53" s="60"/>
-      <c r="E53" s="60"/>
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
@@ -3136,14 +3109,11 @@
       <c r="Z53" s="1"/>
     </row>
     <row r="54" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="17">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="B54" s="55"/>
-      <c r="C54" s="55"/>
-      <c r="D54" s="60"/>
-      <c r="E54" s="60"/>
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
@@ -3167,14 +3137,11 @@
       <c r="Z54" s="1"/>
     </row>
     <row r="55" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="17">
-        <f t="shared" si="0"/>
-        <v>51</v>
-      </c>
-      <c r="B55" s="55"/>
-      <c r="C55" s="55"/>
-      <c r="D55" s="60"/>
-      <c r="E55" s="60"/>
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
@@ -3198,14 +3165,11 @@
       <c r="Z55" s="1"/>
     </row>
     <row r="56" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="17">
-        <f t="shared" si="0"/>
-        <v>52</v>
-      </c>
-      <c r="B56" s="55"/>
-      <c r="C56" s="55"/>
-      <c r="D56" s="60"/>
-      <c r="E56" s="60"/>
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
@@ -3229,76 +3193,67 @@
       <c r="Z56" s="1"/>
     </row>
     <row r="57" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="17">
-        <f t="shared" si="0"/>
-        <v>53</v>
-      </c>
-      <c r="B57" s="55"/>
-      <c r="C57" s="55"/>
-      <c r="D57" s="60"/>
-      <c r="E57" s="60"/>
-      <c r="F57" s="3"/>
-      <c r="G57" s="3"/>
-      <c r="H57" s="3"/>
-      <c r="I57" s="3"/>
-      <c r="J57" s="3"/>
-      <c r="K57" s="3"/>
-      <c r="L57" s="3"/>
-      <c r="M57" s="3"/>
-      <c r="N57" s="3"/>
-      <c r="O57" s="3"/>
-      <c r="P57" s="3"/>
-      <c r="Q57" s="3"/>
-      <c r="R57" s="3"/>
-      <c r="S57" s="3"/>
-      <c r="T57" s="3"/>
-      <c r="U57" s="3"/>
-      <c r="V57" s="3"/>
-      <c r="W57" s="3"/>
-      <c r="X57" s="3"/>
-      <c r="Y57" s="3"/>
-      <c r="Z57" s="3"/>
+      <c r="A57" s="1"/>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1"/>
+      <c r="K57" s="1"/>
+      <c r="L57" s="1"/>
+      <c r="M57" s="1"/>
+      <c r="N57" s="1"/>
+      <c r="O57" s="1"/>
+      <c r="P57" s="1"/>
+      <c r="Q57" s="1"/>
+      <c r="R57" s="1"/>
+      <c r="S57" s="1"/>
+      <c r="T57" s="1"/>
+      <c r="U57" s="1"/>
+      <c r="V57" s="1"/>
+      <c r="W57" s="1"/>
+      <c r="X57" s="1"/>
+      <c r="Y57" s="1"/>
+      <c r="Z57" s="1"/>
     </row>
     <row r="58" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="17">
-        <f t="shared" si="0"/>
-        <v>54</v>
-      </c>
-      <c r="B58" s="55"/>
-      <c r="C58" s="55"/>
-      <c r="D58" s="60"/>
-      <c r="E58" s="60"/>
-      <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
-      <c r="H58" s="1"/>
-      <c r="I58" s="1"/>
-      <c r="J58" s="1"/>
-      <c r="K58" s="1"/>
-      <c r="L58" s="1"/>
-      <c r="M58" s="1"/>
-      <c r="N58" s="1"/>
-      <c r="O58" s="1"/>
-      <c r="P58" s="1"/>
-      <c r="Q58" s="1"/>
-      <c r="R58" s="1"/>
-      <c r="S58" s="1"/>
-      <c r="T58" s="1"/>
-      <c r="U58" s="1"/>
-      <c r="V58" s="1"/>
-      <c r="W58" s="1"/>
-      <c r="X58" s="1"/>
-      <c r="Y58" s="1"/>
-      <c r="Z58" s="1"/>
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="3"/>
+      <c r="G58" s="3"/>
+      <c r="H58" s="3"/>
+      <c r="I58" s="3"/>
+      <c r="J58" s="3"/>
+      <c r="K58" s="3"/>
+      <c r="L58" s="3"/>
+      <c r="M58" s="3"/>
+      <c r="N58" s="3"/>
+      <c r="O58" s="3"/>
+      <c r="P58" s="3"/>
+      <c r="Q58" s="3"/>
+      <c r="R58" s="3"/>
+      <c r="S58" s="3"/>
+      <c r="T58" s="3"/>
+      <c r="U58" s="3"/>
+      <c r="V58" s="3"/>
+      <c r="W58" s="3"/>
+      <c r="X58" s="3"/>
+      <c r="Y58" s="3"/>
+      <c r="Z58" s="3"/>
     </row>
     <row r="59" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="17">
-        <f t="shared" si="0"/>
-        <v>55</v>
-      </c>
-      <c r="B59" s="55"/>
-      <c r="C59" s="55"/>
-      <c r="D59" s="60"/>
-      <c r="E59" s="60"/>
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
@@ -3322,14 +3277,11 @@
       <c r="Z59" s="1"/>
     </row>
     <row r="60" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="17">
-        <f t="shared" si="0"/>
-        <v>56</v>
-      </c>
-      <c r="B60" s="55"/>
-      <c r="C60" s="55"/>
-      <c r="D60" s="60"/>
-      <c r="E60" s="60"/>
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
@@ -3353,14 +3305,11 @@
       <c r="Z60" s="1"/>
     </row>
     <row r="61" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="17">
-        <f t="shared" si="0"/>
-        <v>57</v>
-      </c>
-      <c r="B61" s="55"/>
-      <c r="C61" s="55"/>
-      <c r="D61" s="60"/>
-      <c r="E61" s="60"/>
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
@@ -3384,14 +3333,11 @@
       <c r="Z61" s="1"/>
     </row>
     <row r="62" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="17">
-        <f t="shared" si="0"/>
-        <v>58</v>
-      </c>
-      <c r="B62" s="55"/>
-      <c r="C62" s="55"/>
-      <c r="D62" s="60"/>
-      <c r="E62" s="60"/>
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
@@ -3415,14 +3361,11 @@
       <c r="Z62" s="1"/>
     </row>
     <row r="63" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="17">
-        <f t="shared" si="0"/>
-        <v>59</v>
-      </c>
-      <c r="B63" s="55"/>
-      <c r="C63" s="55"/>
-      <c r="D63" s="60"/>
-      <c r="E63" s="60"/>
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
@@ -3446,14 +3389,11 @@
       <c r="Z63" s="1"/>
     </row>
     <row r="64" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="17">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="B64" s="55"/>
-      <c r="C64" s="55"/>
-      <c r="D64" s="60"/>
-      <c r="E64" s="60"/>
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
       <c r="H64" s="1"/>
@@ -3477,14 +3417,11 @@
       <c r="Z64" s="1"/>
     </row>
     <row r="65" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="17">
-        <f t="shared" si="0"/>
-        <v>61</v>
-      </c>
-      <c r="B65" s="55"/>
-      <c r="C65" s="55"/>
-      <c r="D65" s="60"/>
-      <c r="E65" s="60"/>
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
       <c r="H65" s="1"/>
@@ -3508,14 +3445,11 @@
       <c r="Z65" s="1"/>
     </row>
     <row r="66" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="17">
-        <f t="shared" si="0"/>
-        <v>62</v>
-      </c>
-      <c r="B66" s="55"/>
-      <c r="C66" s="55"/>
-      <c r="D66" s="60"/>
-      <c r="E66" s="60"/>
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
@@ -3539,14 +3473,11 @@
       <c r="Z66" s="1"/>
     </row>
     <row r="67" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="17">
-        <f t="shared" si="0"/>
-        <v>63</v>
-      </c>
-      <c r="B67" s="55"/>
-      <c r="C67" s="55"/>
-      <c r="D67" s="60"/>
-      <c r="E67" s="60"/>
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
       <c r="H67" s="1"/>
@@ -3570,14 +3501,11 @@
       <c r="Z67" s="1"/>
     </row>
     <row r="68" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="17">
-        <f t="shared" si="0"/>
-        <v>64</v>
-      </c>
-      <c r="B68" s="55"/>
-      <c r="C68" s="55"/>
-      <c r="D68" s="60"/>
-      <c r="E68" s="60"/>
+      <c r="A68" s="1"/>
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
       <c r="H68" s="1"/>
@@ -3601,14 +3529,11 @@
       <c r="Z68" s="1"/>
     </row>
     <row r="69" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="17">
-        <f t="shared" si="0"/>
-        <v>65</v>
-      </c>
-      <c r="B69" s="55"/>
-      <c r="C69" s="55"/>
-      <c r="D69" s="60"/>
-      <c r="E69" s="60"/>
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
@@ -3632,14 +3557,11 @@
       <c r="Z69" s="1"/>
     </row>
     <row r="70" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="17">
-        <f t="shared" ref="A70:A79" si="1">ROW(A70) - 4</f>
-        <v>66</v>
-      </c>
-      <c r="B70" s="55"/>
-      <c r="C70" s="55"/>
-      <c r="D70" s="60"/>
-      <c r="E70" s="60"/>
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
       <c r="H70" s="1"/>
@@ -3663,14 +3585,11 @@
       <c r="Z70" s="1"/>
     </row>
     <row r="71" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="17">
-        <f t="shared" si="1"/>
-        <v>67</v>
-      </c>
-      <c r="B71" s="55"/>
-      <c r="C71" s="55"/>
-      <c r="D71" s="60"/>
-      <c r="E71" s="60"/>
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
       <c r="H71" s="1"/>
@@ -3694,14 +3613,11 @@
       <c r="Z71" s="1"/>
     </row>
     <row r="72" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="17">
-        <f t="shared" si="1"/>
-        <v>68</v>
-      </c>
-      <c r="B72" s="55"/>
-      <c r="C72" s="55"/>
-      <c r="D72" s="60"/>
-      <c r="E72" s="60"/>
+      <c r="A72" s="1"/>
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
       <c r="H72" s="1"/>
@@ -3725,14 +3641,11 @@
       <c r="Z72" s="1"/>
     </row>
     <row r="73" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="17">
-        <f t="shared" si="1"/>
-        <v>69</v>
-      </c>
-      <c r="B73" s="55"/>
-      <c r="C73" s="55"/>
-      <c r="D73" s="60"/>
-      <c r="E73" s="60"/>
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
       <c r="H73" s="1"/>
@@ -3756,14 +3669,11 @@
       <c r="Z73" s="1"/>
     </row>
     <row r="74" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="17">
-        <f t="shared" si="1"/>
-        <v>70</v>
-      </c>
-      <c r="B74" s="55"/>
-      <c r="C74" s="55"/>
-      <c r="D74" s="60"/>
-      <c r="E74" s="60"/>
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1"/>
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
       <c r="H74" s="1"/>
@@ -3787,14 +3697,11 @@
       <c r="Z74" s="1"/>
     </row>
     <row r="75" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="17">
-        <f t="shared" si="1"/>
-        <v>71</v>
-      </c>
-      <c r="B75" s="55"/>
-      <c r="C75" s="55"/>
-      <c r="D75" s="60"/>
-      <c r="E75" s="60"/>
+      <c r="A75" s="1"/>
+      <c r="B75" s="1"/>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
       <c r="H75" s="1"/>
@@ -3818,14 +3725,11 @@
       <c r="Z75" s="1"/>
     </row>
     <row r="76" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="17">
-        <f t="shared" si="1"/>
-        <v>72</v>
-      </c>
-      <c r="B76" s="55"/>
-      <c r="C76" s="55"/>
-      <c r="D76" s="60"/>
-      <c r="E76" s="60"/>
+      <c r="A76" s="1"/>
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
       <c r="H76" s="1"/>
@@ -3849,14 +3753,11 @@
       <c r="Z76" s="1"/>
     </row>
     <row r="77" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="17">
-        <f t="shared" si="1"/>
-        <v>73</v>
-      </c>
-      <c r="B77" s="55"/>
-      <c r="C77" s="55"/>
-      <c r="D77" s="60"/>
-      <c r="E77" s="60"/>
+      <c r="A77" s="1"/>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
       <c r="F77" s="1"/>
       <c r="G77" s="1"/>
       <c r="H77" s="1"/>
@@ -3880,14 +3781,11 @@
       <c r="Z77" s="1"/>
     </row>
     <row r="78" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="17">
-        <f t="shared" si="1"/>
-        <v>74</v>
-      </c>
-      <c r="B78" s="55"/>
-      <c r="C78" s="55"/>
-      <c r="D78" s="60"/>
-      <c r="E78" s="60"/>
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
       <c r="F78" s="1"/>
       <c r="G78" s="1"/>
       <c r="H78" s="1"/>
@@ -3910,15 +3808,12 @@
       <c r="Y78" s="1"/>
       <c r="Z78" s="1"/>
     </row>
-    <row r="79" spans="1:26" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="16">
-        <f t="shared" si="1"/>
-        <v>75</v>
-      </c>
-      <c r="B79" s="104"/>
-      <c r="C79" s="105"/>
-      <c r="D79" s="61"/>
-      <c r="E79" s="61"/>
+    <row r="79" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="1"/>
+      <c r="B79" s="1"/>
+      <c r="C79" s="1"/>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1"/>
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
       <c r="H79" s="1"/>
@@ -3941,8 +3836,8 @@
       <c r="Y79" s="1"/>
       <c r="Z79" s="1"/>
     </row>
-    <row r="80" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="50"/>
+    <row r="80" spans="1:26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
@@ -3970,7 +3865,7 @@
       <c r="Z80" s="1"/>
     </row>
     <row r="81" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="10"/>
+      <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
@@ -3998,7 +3893,7 @@
       <c r="Z81" s="1"/>
     </row>
     <row r="82" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="10"/>
+      <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
@@ -4333,8 +4228,8 @@
       <c r="Y93" s="1"/>
       <c r="Z93" s="1"/>
     </row>
-    <row r="94" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="13"/>
+    <row r="94" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="10"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
@@ -4362,7 +4257,7 @@
       <c r="Z94" s="1"/>
     </row>
     <row r="95" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="10"/>
+      <c r="A95" s="13"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
@@ -6685,7 +6580,7 @@
       <c r="Y177" s="1"/>
       <c r="Z177" s="1"/>
     </row>
-    <row r="178" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="10"/>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
@@ -29701,11 +29596,44 @@
       <c r="Y999" s="1"/>
       <c r="Z999" s="1"/>
     </row>
+    <row r="1000" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1000" s="10"/>
+      <c r="B1000" s="1"/>
+      <c r="C1000" s="1"/>
+      <c r="D1000" s="1"/>
+      <c r="E1000" s="1"/>
+      <c r="F1000" s="1"/>
+      <c r="G1000" s="1"/>
+      <c r="H1000" s="1"/>
+      <c r="I1000" s="1"/>
+      <c r="J1000" s="1"/>
+      <c r="K1000" s="1"/>
+      <c r="L1000" s="1"/>
+      <c r="M1000" s="1"/>
+      <c r="N1000" s="1"/>
+      <c r="O1000" s="1"/>
+      <c r="P1000" s="1"/>
+      <c r="Q1000" s="1"/>
+      <c r="R1000" s="1"/>
+      <c r="S1000" s="1"/>
+      <c r="T1000" s="1"/>
+      <c r="U1000" s="1"/>
+      <c r="V1000" s="1"/>
+      <c r="W1000" s="1"/>
+      <c r="X1000" s="1"/>
+      <c r="Y1000" s="1"/>
+      <c r="Z1000" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="8">
+    <mergeCell ref="A17:A22"/>
+    <mergeCell ref="A23:A28"/>
+    <mergeCell ref="A29:E29"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A5:A10"/>
+    <mergeCell ref="A11:A16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -29729,87 +29657,87 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="107" t="s">
+      <c r="A1" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="116"/>
-      <c r="C1" s="116"/>
-      <c r="D1" s="117"/>
+      <c r="B1" s="111"/>
+      <c r="C1" s="111"/>
+      <c r="D1" s="112"/>
     </row>
     <row r="2" spans="1:4" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="113" t="s">
+      <c r="A2" s="108" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="113"/>
+      <c r="C2" s="113"/>
+      <c r="D2" s="114"/>
+    </row>
+    <row r="3" spans="1:4" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="115" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="118"/>
-      <c r="C2" s="118"/>
-      <c r="D2" s="119"/>
-    </row>
-    <row r="3" spans="1:4" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
-        <v>6</v>
+      <c r="C3" s="116"/>
+      <c r="D3" s="25" t="s">
+        <v>33</v>
       </c>
-      <c r="B3" s="120" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="121"/>
-      <c r="D3" s="26" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="4" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
-      <c r="B4" s="28" t="s">
+      <c r="A4" s="26"/>
+      <c r="B4" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="29" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="19"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="18"/>
     </row>
     <row r="6" spans="1:4" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="18"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="17"/>
       <c r="D6" s="5"/>
     </row>
     <row r="7" spans="1:4" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="23"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="22"/>
       <c r="D7" s="5"/>
     </row>
     <row r="8" spans="1:4" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="20"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="19"/>
       <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:4" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="22"/>
-      <c r="C9" s="21"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="20"/>
       <c r="D9" s="7"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="24"/>
+      <c r="A11" s="23"/>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -30812,291 +30740,291 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" style="35" customWidth="1"/>
-    <col min="2" max="2" width="44.5703125" style="35" customWidth="1"/>
-    <col min="3" max="3" width="50" style="35" customWidth="1"/>
-    <col min="4" max="5" width="20.7109375" style="35" customWidth="1"/>
-    <col min="6" max="9" width="32.28515625" style="35" customWidth="1"/>
-    <col min="10" max="26" width="8.85546875" style="35" customWidth="1"/>
-    <col min="27" max="16384" width="14.42578125" style="35"/>
+    <col min="1" max="1" width="20.42578125" style="34" customWidth="1"/>
+    <col min="2" max="2" width="44.5703125" style="34" customWidth="1"/>
+    <col min="3" max="3" width="50" style="34" customWidth="1"/>
+    <col min="4" max="5" width="20.7109375" style="34" customWidth="1"/>
+    <col min="6" max="9" width="32.28515625" style="34" customWidth="1"/>
+    <col min="10" max="26" width="8.85546875" style="34" customWidth="1"/>
+    <col min="27" max="16384" width="14.42578125" style="34"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="107" t="s">
+      <c r="A1" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="116"/>
-      <c r="C1" s="116"/>
-      <c r="D1" s="116"/>
-      <c r="E1" s="117"/>
+      <c r="B1" s="111"/>
+      <c r="C1" s="111"/>
+      <c r="D1" s="111"/>
+      <c r="E1" s="112"/>
     </row>
     <row r="2" spans="1:9" ht="75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="113" t="s">
-        <v>33</v>
+      <c r="A2" s="108" t="s">
+        <v>31</v>
       </c>
-      <c r="B2" s="118"/>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="119"/>
+      <c r="B2" s="113"/>
+      <c r="C2" s="113"/>
+      <c r="D2" s="113"/>
+      <c r="E2" s="114"/>
     </row>
     <row r="3" spans="1:9" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="44"/>
-      <c r="B3" s="28" t="s">
+      <c r="A3" s="43"/>
+      <c r="B3" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="49" t="s">
-        <v>30</v>
+      <c r="D3" s="48" t="s">
+        <v>28</v>
       </c>
-      <c r="E3" s="49" t="s">
-        <v>31</v>
+      <c r="E3" s="48" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
     </row>
     <row r="5" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
     </row>
     <row r="6" spans="1:9" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="47" t="s">
+      <c r="A6" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
     </row>
     <row r="7" spans="1:9" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="106"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="101"/>
     </row>
     <row r="8" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="40"/>
-      <c r="B9" s="40"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="41"/>
+      <c r="A9" s="39"/>
+      <c r="B9" s="39"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="40"/>
     </row>
     <row r="10" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="48"/>
+      <c r="A10" s="47"/>
     </row>
     <row r="11" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="42"/>
-      <c r="C14" s="43"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="42"/>
-      <c r="I14" s="43"/>
+      <c r="B14" s="41"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="42"/>
     </row>
     <row r="15" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="42"/>
-      <c r="C15" s="43"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="43"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="43"/>
+      <c r="B15" s="41"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="42"/>
     </row>
     <row r="16" spans="1:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="42"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="43"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="43"/>
+      <c r="B16" s="41"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="42"/>
     </row>
     <row r="17" spans="2:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="42"/>
-      <c r="C17" s="43"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="43"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="43"/>
+      <c r="B17" s="41"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="42"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="42"/>
     </row>
     <row r="18" spans="2:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="42"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="43"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="43"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="43"/>
+      <c r="B18" s="41"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="42"/>
     </row>
     <row r="19" spans="2:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="42"/>
-      <c r="C19" s="43"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="43"/>
-      <c r="F19" s="42"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="42"/>
-      <c r="I19" s="43"/>
+      <c r="B19" s="41"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="42"/>
     </row>
     <row r="20" spans="2:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="42"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="43"/>
-      <c r="F20" s="42"/>
-      <c r="G20" s="43"/>
-      <c r="H20" s="42"/>
-      <c r="I20" s="43"/>
+      <c r="B20" s="41"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="42"/>
     </row>
     <row r="21" spans="2:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="42"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="42"/>
-      <c r="I21" s="43"/>
+      <c r="B21" s="41"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="41"/>
+      <c r="I21" s="42"/>
     </row>
     <row r="22" spans="2:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="42"/>
-      <c r="C22" s="43"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="43"/>
-      <c r="F22" s="42"/>
-      <c r="G22" s="43"/>
-      <c r="H22" s="42"/>
-      <c r="I22" s="43"/>
+      <c r="B22" s="41"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="41"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="41"/>
+      <c r="I22" s="42"/>
     </row>
     <row r="23" spans="2:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="42"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="42"/>
-      <c r="G23" s="43"/>
-      <c r="H23" s="42"/>
-      <c r="I23" s="43"/>
+      <c r="B23" s="41"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="41"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="41"/>
+      <c r="I23" s="42"/>
     </row>
     <row r="24" spans="2:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="42"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="42"/>
-      <c r="G24" s="43"/>
-      <c r="H24" s="42"/>
-      <c r="I24" s="43"/>
+      <c r="B24" s="41"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="41"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="41"/>
+      <c r="I24" s="42"/>
     </row>
     <row r="25" spans="2:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="42"/>
-      <c r="C25" s="43"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="43"/>
-      <c r="F25" s="42"/>
-      <c r="G25" s="43"/>
-      <c r="H25" s="42"/>
-      <c r="I25" s="43"/>
+      <c r="B25" s="41"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="41"/>
+      <c r="G25" s="42"/>
+      <c r="H25" s="41"/>
+      <c r="I25" s="42"/>
     </row>
     <row r="26" spans="2:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="42"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="43"/>
-      <c r="F26" s="42"/>
-      <c r="G26" s="43"/>
-      <c r="H26" s="42"/>
-      <c r="I26" s="43"/>
+      <c r="B26" s="41"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="41"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="41"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="41"/>
+      <c r="I26" s="42"/>
     </row>
     <row r="27" spans="2:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="42"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="43"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="43"/>
+      <c r="B27" s="41"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="41"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="41"/>
+      <c r="I27" s="42"/>
     </row>
     <row r="28" spans="2:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="42"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="42"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="42"/>
-      <c r="I28" s="43"/>
+      <c r="B28" s="41"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="41"/>
+      <c r="G28" s="42"/>
+      <c r="H28" s="41"/>
+      <c r="I28" s="42"/>
     </row>
     <row r="29" spans="2:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="42"/>
-      <c r="C29" s="43"/>
-      <c r="D29" s="42"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="42"/>
-      <c r="G29" s="43"/>
-      <c r="H29" s="42"/>
-      <c r="I29" s="43"/>
+      <c r="B29" s="41"/>
+      <c r="C29" s="42"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="42"/>
+      <c r="F29" s="41"/>
+      <c r="G29" s="42"/>
+      <c r="H29" s="41"/>
+      <c r="I29" s="42"/>
     </row>
     <row r="30" spans="2:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="42"/>
-      <c r="C30" s="43"/>
-      <c r="D30" s="42"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="42"/>
-      <c r="G30" s="43"/>
-      <c r="H30" s="42"/>
-      <c r="I30" s="43"/>
+      <c r="B30" s="41"/>
+      <c r="C30" s="42"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="42"/>
+      <c r="F30" s="41"/>
+      <c r="G30" s="42"/>
+      <c r="H30" s="41"/>
+      <c r="I30" s="42"/>
     </row>
     <row r="31" spans="2:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="42"/>
-      <c r="C31" s="43"/>
-      <c r="D31" s="42"/>
-      <c r="E31" s="43"/>
-      <c r="F31" s="42"/>
-      <c r="G31" s="43"/>
-      <c r="H31" s="42"/>
-      <c r="I31" s="43"/>
+      <c r="B31" s="41"/>
+      <c r="C31" s="42"/>
+      <c r="D31" s="41"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="41"/>
+      <c r="G31" s="42"/>
+      <c r="H31" s="41"/>
+      <c r="I31" s="42"/>
     </row>
     <row r="32" spans="2:9" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="42"/>
-      <c r="C32" s="43"/>
-      <c r="D32" s="42"/>
-      <c r="E32" s="43"/>
-      <c r="F32" s="42"/>
-      <c r="G32" s="43"/>
-      <c r="H32" s="42"/>
-      <c r="I32" s="43"/>
+      <c r="B32" s="41"/>
+      <c r="C32" s="42"/>
+      <c r="D32" s="41"/>
+      <c r="E32" s="42"/>
+      <c r="F32" s="41"/>
+      <c r="G32" s="42"/>
+      <c r="H32" s="41"/>
+      <c r="I32" s="42"/>
     </row>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -32086,467 +32014,448 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" style="35" customWidth="1"/>
-    <col min="2" max="3" width="40.7109375" style="35" customWidth="1"/>
-    <col min="4" max="6" width="20.7109375" style="35" customWidth="1"/>
-    <col min="7" max="7" width="26.85546875" style="35" customWidth="1"/>
-    <col min="8" max="26" width="8.85546875" style="35" customWidth="1"/>
-    <col min="27" max="16384" width="14.42578125" style="35"/>
+    <col min="1" max="1" width="26.85546875" style="34" customWidth="1"/>
+    <col min="2" max="3" width="40.7109375" style="34" customWidth="1"/>
+    <col min="4" max="6" width="20.7109375" style="34" customWidth="1"/>
+    <col min="7" max="7" width="26.85546875" style="34" customWidth="1"/>
+    <col min="8" max="26" width="8.85546875" style="34" customWidth="1"/>
+    <col min="27" max="16384" width="14.42578125" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="71" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="124" t="s">
+    <row r="1" spans="1:7" s="67" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="119" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="124"/>
-      <c r="C1" s="124"/>
-      <c r="D1" s="124"/>
-      <c r="E1" s="124"/>
-      <c r="F1" s="125"/>
-      <c r="G1" s="70"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="120"/>
+      <c r="G1" s="66"/>
     </row>
     <row r="2" spans="1:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="113" t="s">
-        <v>40</v>
+      <c r="A2" s="108" t="s">
+        <v>38</v>
       </c>
-      <c r="B2" s="114"/>
-      <c r="C2" s="114"/>
-      <c r="D2" s="114"/>
-      <c r="E2" s="114"/>
-      <c r="F2" s="123"/>
+      <c r="B2" s="109"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
+      <c r="F2" s="118"/>
     </row>
     <row r="3" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="122" t="s">
+      <c r="A3" s="117" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="117"/>
+      <c r="C3" s="117"/>
+      <c r="D3" s="117"/>
+      <c r="E3" s="117"/>
+      <c r="F3" s="117"/>
+    </row>
+    <row r="4" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="62" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="63" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="64" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="64" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="65" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="95" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="90"/>
+      <c r="C5" s="77"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="69"/>
+    </row>
+    <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="96" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="91"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="70"/>
+    </row>
+    <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="96" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="79"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="70"/>
+    </row>
+    <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="97" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="81"/>
+      <c r="C8" s="82"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="73"/>
+    </row>
+    <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="97" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="79"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="73"/>
+    </row>
+    <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="97" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="79"/>
+      <c r="C10" s="80"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="73"/>
+    </row>
+    <row r="11" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="117" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="117"/>
+      <c r="C11" s="117"/>
+      <c r="D11" s="117"/>
+      <c r="E11" s="117"/>
+      <c r="F11" s="117"/>
+    </row>
+    <row r="12" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="62" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="63" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="64" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="64" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="65" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="95" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="92"/>
+      <c r="C13" s="83"/>
+      <c r="D13" s="68"/>
+      <c r="E13" s="68"/>
+      <c r="F13" s="55"/>
+    </row>
+    <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="96" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="93"/>
+      <c r="C14" s="84"/>
+      <c r="D14" s="54"/>
+      <c r="E14" s="54"/>
+      <c r="F14" s="74"/>
+    </row>
+    <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="96" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="85"/>
+      <c r="C15" s="86"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="74"/>
+    </row>
+    <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="97" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="87"/>
+      <c r="C16" s="88"/>
+      <c r="D16" s="71"/>
+      <c r="E16" s="72"/>
+      <c r="F16" s="57"/>
+    </row>
+    <row r="17" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="97" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="85"/>
+      <c r="C17" s="86"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="57"/>
+    </row>
+    <row r="18" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="97" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="85"/>
+      <c r="C18" s="86"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="57"/>
+    </row>
+    <row r="19" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="117" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="122"/>
-      <c r="C3" s="122"/>
-      <c r="D3" s="122"/>
-      <c r="E3" s="122"/>
-      <c r="F3" s="122"/>
-    </row>
-    <row r="4" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="66" t="s">
+      <c r="B19" s="117"/>
+      <c r="C19" s="117"/>
+      <c r="D19" s="117"/>
+      <c r="E19" s="117"/>
+      <c r="F19" s="117"/>
+    </row>
+    <row r="20" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B20" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="67" t="s">
+      <c r="C20" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="68" t="s">
+      <c r="D20" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="68" t="s">
+      <c r="E20" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="69" t="s">
-        <v>41</v>
+      <c r="F20" s="65" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="99" t="s">
+    <row r="21" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="95" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="94"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="73"/>
-    </row>
-    <row r="6" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="100" t="s">
+      <c r="B21" s="92"/>
+      <c r="C21" s="83"/>
+      <c r="D21" s="68"/>
+      <c r="E21" s="68"/>
+      <c r="F21" s="55"/>
+    </row>
+    <row r="22" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="96" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="95"/>
-      <c r="C6" s="82"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="74"/>
-    </row>
-    <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="100" t="s">
+      <c r="B22" s="93"/>
+      <c r="C22" s="84"/>
+      <c r="D22" s="54"/>
+      <c r="E22" s="54"/>
+      <c r="F22" s="74"/>
+    </row>
+    <row r="23" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="96" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="83"/>
-      <c r="C7" s="84"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="74"/>
-    </row>
-    <row r="8" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="101" t="s">
+      <c r="B23" s="85"/>
+      <c r="C23" s="86"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="74"/>
+    </row>
+    <row r="24" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="97" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="85"/>
-      <c r="C8" s="86"/>
-      <c r="D8" s="75"/>
-      <c r="E8" s="76"/>
-      <c r="F8" s="77"/>
-    </row>
-    <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="101" t="s">
+      <c r="B24" s="87"/>
+      <c r="C24" s="88"/>
+      <c r="D24" s="71"/>
+      <c r="E24" s="72"/>
+      <c r="F24" s="57"/>
+    </row>
+    <row r="25" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="97" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="83"/>
-      <c r="C9" s="84"/>
-      <c r="D9" s="58"/>
-      <c r="E9" s="58"/>
-      <c r="F9" s="77"/>
-    </row>
-    <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="101" t="s">
+      <c r="B25" s="85"/>
+      <c r="C25" s="86"/>
+      <c r="D25" s="56"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="57"/>
+    </row>
+    <row r="26" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="97" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="83"/>
-      <c r="C10" s="84"/>
-      <c r="D10" s="58"/>
-      <c r="E10" s="58"/>
-      <c r="F10" s="77"/>
-    </row>
-    <row r="11" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="122" t="s">
+      <c r="B26" s="85"/>
+      <c r="C26" s="86"/>
+      <c r="D26" s="56"/>
+      <c r="E26" s="56"/>
+      <c r="F26" s="57"/>
+    </row>
+    <row r="27" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="117" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="122"/>
-      <c r="C11" s="122"/>
-      <c r="D11" s="122"/>
-      <c r="E11" s="122"/>
-      <c r="F11" s="122"/>
-    </row>
-    <row r="12" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="66" t="s">
+      <c r="B27" s="117"/>
+      <c r="C27" s="117"/>
+      <c r="D27" s="117"/>
+      <c r="E27" s="117"/>
+      <c r="F27" s="117"/>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B28" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="67" t="s">
+      <c r="C28" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="68" t="s">
+      <c r="D28" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="68" t="s">
+      <c r="E28" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="69" t="s">
-        <v>41</v>
+      <c r="F28" s="65" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="99" t="s">
+    <row r="29" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="95" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="96"/>
-      <c r="C13" s="87"/>
-      <c r="D13" s="72"/>
-      <c r="E13" s="72"/>
-      <c r="F13" s="57"/>
-    </row>
-    <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="100" t="s">
+      <c r="B29" s="92"/>
+      <c r="C29" s="83"/>
+      <c r="D29" s="68"/>
+      <c r="E29" s="68"/>
+      <c r="F29" s="55"/>
+    </row>
+    <row r="30" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="96" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="97"/>
-      <c r="C14" s="88"/>
-      <c r="D14" s="56"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="78"/>
-    </row>
-    <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="100" t="s">
+      <c r="B30" s="93"/>
+      <c r="C30" s="84"/>
+      <c r="D30" s="54"/>
+      <c r="E30" s="54"/>
+      <c r="F30" s="74"/>
+    </row>
+    <row r="31" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="96" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="89"/>
-      <c r="C15" s="90"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="78"/>
-    </row>
-    <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="101" t="s">
+      <c r="B31" s="85"/>
+      <c r="C31" s="86"/>
+      <c r="D31" s="54"/>
+      <c r="E31" s="54"/>
+      <c r="F31" s="74"/>
+    </row>
+    <row r="32" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="97" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="91"/>
-      <c r="C16" s="92"/>
-      <c r="D16" s="75"/>
-      <c r="E16" s="76"/>
-      <c r="F16" s="59"/>
-    </row>
-    <row r="17" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="101" t="s">
+      <c r="B32" s="87"/>
+      <c r="C32" s="88"/>
+      <c r="D32" s="71"/>
+      <c r="E32" s="72"/>
+      <c r="F32" s="57"/>
+    </row>
+    <row r="33" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="97" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="89"/>
-      <c r="C17" s="90"/>
-      <c r="D17" s="58"/>
-      <c r="E17" s="58"/>
-      <c r="F17" s="59"/>
-    </row>
-    <row r="18" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="101" t="s">
+      <c r="B33" s="85"/>
+      <c r="C33" s="86"/>
+      <c r="D33" s="56"/>
+      <c r="E33" s="56"/>
+      <c r="F33" s="57"/>
+    </row>
+    <row r="34" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="98" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="89"/>
-      <c r="C18" s="90"/>
-      <c r="D18" s="58"/>
-      <c r="E18" s="58"/>
-      <c r="F18" s="59"/>
-    </row>
-    <row r="19" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="122" t="s">
-        <v>38</v>
+      <c r="B34" s="94"/>
+      <c r="C34" s="89"/>
+      <c r="D34" s="75"/>
+      <c r="E34" s="75"/>
+      <c r="F34" s="76"/>
+    </row>
+    <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="60"/>
+    </row>
+    <row r="36" spans="1:6" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="117" t="s">
+        <v>23</v>
       </c>
-      <c r="B19" s="122"/>
-      <c r="C19" s="122"/>
-      <c r="D19" s="122"/>
-      <c r="E19" s="122"/>
-      <c r="F19" s="122"/>
-    </row>
-    <row r="20" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="66" t="s">
-        <v>18</v>
+      <c r="B36" s="117"/>
+      <c r="C36" s="117"/>
+    </row>
+    <row r="37" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="99" t="s">
+        <v>27</v>
       </c>
-      <c r="B20" s="29" t="s">
+      <c r="B37" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="67" t="s">
+      <c r="C37" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="68" t="s">
-        <v>19</v>
-      </c>
-      <c r="E20" s="68" t="s">
-        <v>20</v>
-      </c>
-      <c r="F20" s="69" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="99" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="96"/>
-      <c r="C21" s="87"/>
-      <c r="D21" s="72"/>
-      <c r="E21" s="72"/>
-      <c r="F21" s="57"/>
-    </row>
-    <row r="22" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="100" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="97"/>
-      <c r="C22" s="88"/>
-      <c r="D22" s="56"/>
-      <c r="E22" s="56"/>
-      <c r="F22" s="78"/>
-    </row>
-    <row r="23" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="100" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" s="89"/>
-      <c r="C23" s="90"/>
-      <c r="D23" s="56"/>
-      <c r="E23" s="56"/>
-      <c r="F23" s="78"/>
-    </row>
-    <row r="24" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="101" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" s="91"/>
-      <c r="C24" s="92"/>
-      <c r="D24" s="75"/>
-      <c r="E24" s="76"/>
-      <c r="F24" s="59"/>
-    </row>
-    <row r="25" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="101" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" s="89"/>
-      <c r="C25" s="90"/>
-      <c r="D25" s="58"/>
-      <c r="E25" s="58"/>
-      <c r="F25" s="59"/>
-    </row>
-    <row r="26" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="101" t="s">
-        <v>22</v>
-      </c>
-      <c r="B26" s="89"/>
-      <c r="C26" s="90"/>
-      <c r="D26" s="58"/>
-      <c r="E26" s="58"/>
-      <c r="F26" s="59"/>
-    </row>
-    <row r="27" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="122" t="s">
-        <v>39</v>
-      </c>
-      <c r="B27" s="122"/>
-      <c r="C27" s="122"/>
-      <c r="D27" s="122"/>
-      <c r="E27" s="122"/>
-      <c r="F27" s="122"/>
-    </row>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="66" t="s">
-        <v>18</v>
-      </c>
-      <c r="B28" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="C28" s="67" t="s">
-        <v>2</v>
-      </c>
-      <c r="D28" s="68" t="s">
-        <v>19</v>
-      </c>
-      <c r="E28" s="68" t="s">
-        <v>20</v>
-      </c>
-      <c r="F28" s="69" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="99" t="s">
-        <v>21</v>
-      </c>
-      <c r="B29" s="96"/>
-      <c r="C29" s="87"/>
-      <c r="D29" s="72"/>
-      <c r="E29" s="72"/>
-      <c r="F29" s="57"/>
-    </row>
-    <row r="30" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="100" t="s">
-        <v>21</v>
-      </c>
-      <c r="B30" s="97"/>
-      <c r="C30" s="88"/>
-      <c r="D30" s="56"/>
-      <c r="E30" s="56"/>
-      <c r="F30" s="78"/>
-    </row>
-    <row r="31" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="100" t="s">
-        <v>21</v>
-      </c>
-      <c r="B31" s="89"/>
-      <c r="C31" s="90"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="56"/>
-      <c r="F31" s="78"/>
-    </row>
-    <row r="32" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="101" t="s">
-        <v>22</v>
-      </c>
-      <c r="B32" s="91"/>
-      <c r="C32" s="92"/>
-      <c r="D32" s="75"/>
-      <c r="E32" s="76"/>
-      <c r="F32" s="59"/>
-    </row>
-    <row r="33" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="101" t="s">
-        <v>22</v>
-      </c>
-      <c r="B33" s="89"/>
-      <c r="C33" s="90"/>
-      <c r="D33" s="58"/>
-      <c r="E33" s="58"/>
-      <c r="F33" s="59"/>
-    </row>
-    <row r="34" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="102" t="s">
-        <v>22</v>
-      </c>
-      <c r="B34" s="98"/>
-      <c r="C34" s="93"/>
-      <c r="D34" s="79"/>
-      <c r="E34" s="79"/>
-      <c r="F34" s="80"/>
-    </row>
-    <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="63"/>
-      <c r="B35" s="64"/>
-      <c r="C35" s="64"/>
-      <c r="D35" s="64"/>
-      <c r="E35" s="64"/>
-      <c r="F35" s="64"/>
-    </row>
-    <row r="36" spans="1:7" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="122" t="s">
-        <v>23</v>
-      </c>
-      <c r="B36" s="122"/>
-      <c r="C36" s="122"/>
-      <c r="D36" s="64"/>
-      <c r="E36" s="64"/>
-      <c r="F36" s="64"/>
-    </row>
-    <row r="37" spans="1:7" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="103" t="s">
-        <v>28</v>
-      </c>
-      <c r="B37" s="67" t="s">
-        <v>1</v>
-      </c>
-      <c r="C37" s="68" t="s">
-        <v>2</v>
-      </c>
-      <c r="D37" s="64"/>
-      <c r="E37" s="64"/>
-      <c r="F37" s="64"/>
-    </row>
-    <row r="38" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="99" t="s">
+    </row>
+    <row r="38" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="95" t="s">
         <v>24</v>
       </c>
-      <c r="B38" s="62"/>
-      <c r="C38" s="62"/>
-      <c r="D38" s="65"/>
-      <c r="E38" s="64"/>
-      <c r="F38" s="64"/>
-    </row>
-    <row r="39" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="101" t="s">
+      <c r="B38" s="59"/>
+      <c r="C38" s="59"/>
+      <c r="D38" s="61"/>
+    </row>
+    <row r="39" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="97" t="s">
         <v>25</v>
       </c>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
-      <c r="D39" s="65"/>
-      <c r="E39" s="64"/>
-      <c r="F39" s="64"/>
-      <c r="G39" s="64"/>
-    </row>
-    <row r="40" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D39" s="61"/>
+    </row>
+    <row r="40" spans="1:6" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="9" t="s">
         <v>26</v>
       </c>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
-      <c r="D40" s="65"/>
-      <c r="E40" s="64"/>
-      <c r="F40" s="64"/>
-      <c r="G40" s="64"/>
-    </row>
-    <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="46" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="47" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="D40" s="61"/>
+    </row>
+    <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>